<commit_message>
minor mods to coords file and visuals added
</commit_message>
<xml_diff>
--- a/tomfebn.xlsx
+++ b/tomfebn.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alolinco/Desktop/Research/tom-fe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5289C5FF-B228-6E4D-A85C-AA568E93189E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBB809B-750F-B840-8FA7-013E467ABB6F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="660" windowWidth="24240" windowHeight="19940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2140" yWindow="600" windowWidth="24240" windowHeight="19940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="UTD sheet" sheetId="2" r:id="rId2"/>
     <sheet name="Fall 2018 coords" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Posthess05" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_2018_1fe03_coordinates" localSheetId="1">'UTD sheet'!$AB$1:$AI$73</definedName>
     <definedName name="_2018.06.15_coordinates" localSheetId="1">'UTD sheet'!$W$3:$AC$76</definedName>
     <definedName name="fedft05_coords" localSheetId="2">'Fall 2018 coords'!$P$2:$Y$74</definedName>
-    <definedName name="feopt05_6311g_coords" localSheetId="3">Sheet2!$A$1:$J$72</definedName>
     <definedName name="feopt05_coords" localSheetId="1">'UTD sheet'!$CS$3:$DB$75</definedName>
     <definedName name="fescf02_631g_coor" localSheetId="1">'UTD sheet'!$AV$3:$BD$74</definedName>
     <definedName name="fescf04_coords" localSheetId="1">'UTD sheet'!$BK$3:$BT$74</definedName>
@@ -105,29 +104,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{AE60ED89-89EE-D647-AC36-34EE68D47419}" name="feopt05_6311g_coords" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt6311g/feopt05_6311g_coords.rtf" space="1" consecutive="1" delimiter="\">
-      <textFields count="16">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="5" xr16:uid="{42CE4C14-EBE0-BD4E-A456-3B2BC2FCB249}" name="feopt05_coords" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{42CE4C14-EBE0-BD4E-A456-3B2BC2FCB249}" name="feopt05_coords" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/fe_opt05_20180830/feopt05_coords.rtf" space="1" consecutive="1" delimiter="\">
       <textFields count="16">
         <textField/>
@@ -149,7 +126,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{02AA09EE-88A3-0146-8F71-2D458CA775EB}" name="fescf02_631g_coor" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="5" xr16:uid="{02AA09EE-88A3-0146-8F71-2D458CA775EB}" name="fescf02_631g_coor" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/fescf02/fescf02_631g_coor.rtf" space="1" consecutive="1">
       <textFields count="10">
         <textField/>
@@ -165,7 +142,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" xr16:uid="{4F88F51A-9ACF-0043-97FB-09DD6C883B08}" name="fescf04_coords" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="6" xr16:uid="{4F88F51A-9ACF-0043-97FB-09DD6C883B08}" name="fescf04_coords" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/fescf04_coords.rtf" space="1" consecutive="1" delimiter="\">
       <textFields count="16">
         <textField/>
@@ -187,7 +164,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" xr16:uid="{AF90CF41-864B-284F-9638-9593176733EF}" name="fescf04_s30_coords" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="7" xr16:uid="{AF90CF41-864B-284F-9638-9593176733EF}" name="fescf04_s30_coords" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/fescf04_s30_coords.rtf" space="1" consecutive="1" delimiter="\">
       <textFields count="16">
         <textField/>
@@ -209,7 +186,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" xr16:uid="{8EDD7A7A-542F-9E4D-95A4-33BD898C8051}" name="fescf04_s35_coords" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="8" xr16:uid="{8EDD7A7A-542F-9E4D-95A4-33BD898C8051}" name="fescf04_s35_coords" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/fescf04_s35_coords.rtf" space="1" consecutive="1" delimiter="\">
       <textFields count="16">
         <textField/>
@@ -231,7 +208,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" xr16:uid="{D01B20FA-C2DD-FE45-AB19-569113F1FBAE}" name="fescf05" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="9" xr16:uid="{D01B20FA-C2DD-FE45-AB19-569113F1FBAE}" name="fescf05" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/fescf05.rtf" delimiter="\">
       <textFields count="16">
         <textField/>
@@ -253,7 +230,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" xr16:uid="{C8DD9D3E-BD82-1B43-A5AF-C6A1AACF6A4E}" name="fescf051" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="10" xr16:uid="{C8DD9D3E-BD82-1B43-A5AF-C6A1AACF6A4E}" name="fescf051" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/fescf05.rtf" space="1" consecutive="1" delimiter="\">
       <textFields count="16">
         <textField/>
@@ -275,7 +252,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="run1_coordinates_end" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="run1_coordinates_end" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt6311+g-star/run1/run1_coordinates_end.rtf" space="1" consecutive="1">
       <textFields count="10">
         <textField/>
@@ -291,7 +268,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="testtomfe" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="testtomfe" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/tomfebn_1fe/tomfe_6311+g*.rtf" tab="0" space="1" consecutive="1">
       <textFields count="8">
         <textField/>
@@ -305,7 +282,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="tomfe_6311+g*" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="13" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="tomfe_6311+g*" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/tomfebn_1fe/tomfe_6311+g*.rtf" space="1" consecutive="1">
       <textFields count="10">
         <textField/>
@@ -321,7 +298,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="tomfe_631g" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="14" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="tomfe_631g" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/tomfebn_1fe/tomfe_6311+g*.rtf" space="1" consecutive="1">
       <textFields count="7">
         <textField/>
@@ -334,7 +311,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="tomfe1-02coor" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="15" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="tomfe1-02coor" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/tomfebn_1fe/tomfe1-02coor.rtf" tab="0" space="1" consecutive="1">
       <textFields count="10">
         <textField/>
@@ -350,7 +327,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="tomfebn_start02" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="16" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="tomfebn_start02" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr firstRow="8" sourceFile="/Users/alolinco/Desktop/Research/tom-fe/tomfe_opt631g/tomfebn_1fe/tomfebn_start02.rtf" space="1" consecutive="1">
       <textFields count="7">
         <textField/>
@@ -367,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="301">
   <si>
     <t>Fe</t>
   </si>
@@ -952,13 +929,331 @@
   </si>
   <si>
     <t>6311g</t>
+  </si>
+  <si>
+    <t>6311+g*</t>
+  </si>
+  <si>
+    <t>Used for fe_hess05</t>
+  </si>
+  <si>
+    <t>feopt06</t>
+  </si>
+  <si>
+    <t>Fe      0.05308431     1.28052580     0.31234351</t>
+  </si>
+  <si>
+    <t>B     -0.30543610    -1.82500458    -0.04728875</t>
+  </si>
+  <si>
+    <t>C     -2.02981639     0.69045991     3.44829655</t>
+  </si>
+  <si>
+    <t>H     -1.49328327    -0.19829065     3.79330754</t>
+  </si>
+  <si>
+    <t>H     -2.84520841     0.89073908     4.15147495</t>
+  </si>
+  <si>
+    <t>H     -1.33663154     1.53179979     3.47523117</t>
+  </si>
+  <si>
+    <t>C     -2.58026409     0.47248098     2.04016471</t>
+  </si>
+  <si>
+    <t>C     -3.41571760     1.65567064     1.57853699</t>
+  </si>
+  <si>
+    <t>H     -2.84088135     2.58341360     1.62685645</t>
+  </si>
+  <si>
+    <t>H     -4.29843140     1.77881360     2.21440434</t>
+  </si>
+  <si>
+    <t>H     -3.75343156     1.51535022     0.54797810</t>
+  </si>
+  <si>
+    <t>C     -3.35821819    -0.84951830     1.95870149</t>
+  </si>
+  <si>
+    <t>H     -3.69690561    -1.22527266     2.92543292</t>
+  </si>
+  <si>
+    <t>H     -4.21029520    -0.79377538     1.27204335</t>
+  </si>
+  <si>
+    <t>C     -1.42430770    -1.07175994     0.86894536</t>
+  </si>
+  <si>
+    <t>C      0.84463269     1.56450140    -3.25360823</t>
+  </si>
+  <si>
+    <t>H      0.95358723     2.47164655    -2.65483832</t>
+  </si>
+  <si>
+    <t>H      0.78632486     1.86287880    -4.30574751</t>
+  </si>
+  <si>
+    <t>H      1.74347472     0.95600414    -3.12040591</t>
+  </si>
+  <si>
+    <t>C     -0.39893931     0.78359532    -2.85072994</t>
+  </si>
+  <si>
+    <t>C     -1.65219903     1.64262843    -2.98555470</t>
+  </si>
+  <si>
+    <t>H     -2.54119515     1.08221853    -2.68203712</t>
+  </si>
+  <si>
+    <t>H     -1.78834593     1.96629846    -4.02274370</t>
+  </si>
+  <si>
+    <t>H     -1.57746696     2.53641272    -2.36117435</t>
+  </si>
+  <si>
+    <t>C     -0.52638602    -0.53760219    -3.63699341</t>
+  </si>
+  <si>
+    <t>H     -1.44321263    -0.60385567    -4.22759104</t>
+  </si>
+  <si>
+    <t>H      0.33189657    -0.73049623    -4.28665161</t>
+  </si>
+  <si>
+    <t>C     -0.38860959    -0.98677170    -1.44084942</t>
+  </si>
+  <si>
+    <t>C      3.29372048     0.63657683     2.31440568</t>
+  </si>
+  <si>
+    <t>H      3.15758872     1.70162332     2.11941695</t>
+  </si>
+  <si>
+    <t>H      4.32988358     0.48817369     2.63638997</t>
+  </si>
+  <si>
+    <t>H      2.63465738     0.35726848     3.14056206</t>
+  </si>
+  <si>
+    <t>C      2.99838853    -0.20076206     1.07923770</t>
+  </si>
+  <si>
+    <t>C      3.82464099     0.26684225    -0.11712010</t>
+  </si>
+  <si>
+    <t>H      3.67182612    -0.39571589    -0.97414732</t>
+  </si>
+  <si>
+    <t>H      4.89288902     0.27347112     0.12424092</t>
+  </si>
+  <si>
+    <t>H      3.53359032     1.27579296    -0.41912892</t>
+  </si>
+  <si>
+    <t>C      3.21251750    -1.69851983     1.35613990</t>
+  </si>
+  <si>
+    <t>H      4.10437822    -2.11410785     0.88339460</t>
+  </si>
+  <si>
+    <t>H      3.23365521    -1.92789257     2.42703581</t>
+  </si>
+  <si>
+    <t>C      1.15902996    -1.38021958     0.53258586</t>
+  </si>
+  <si>
+    <t>C     -0.51999038    -3.42183757    -0.06233851</t>
+  </si>
+  <si>
+    <t>C     -0.89046019    -4.17411566    -1.18268251</t>
+  </si>
+  <si>
+    <t>H     -1.02570987    -3.68213511    -2.13863230</t>
+  </si>
+  <si>
+    <t>C     -1.08971488    -5.55165482    -1.11062253</t>
+  </si>
+  <si>
+    <t>H     -1.37601495    -6.09995079    -2.00486612</t>
+  </si>
+  <si>
+    <t>C     -0.92615682    -6.22366047     0.09284243</t>
+  </si>
+  <si>
+    <t>H     -1.08049071    -7.29786015     0.15070476</t>
+  </si>
+  <si>
+    <t>C     -0.56161803    -5.50104666     1.22480547</t>
+  </si>
+  <si>
+    <t>H     -0.43036148    -6.00941515     2.17682648</t>
+  </si>
+  <si>
+    <t>C     -0.36559823    -4.12912369     1.13957071</t>
+  </si>
+  <si>
+    <t>H     -0.08123415    -3.59226656     2.04220247</t>
+  </si>
+  <si>
+    <t>C      0.15497482     2.85603738     1.54666448</t>
+  </si>
+  <si>
+    <t>H     -0.80400574     3.16507983     1.96869707</t>
+  </si>
+  <si>
+    <t>H      0.91686392     2.81873012     2.32636642</t>
+  </si>
+  <si>
+    <t>C      0.52134562     3.62667799     0.36195213</t>
+  </si>
+  <si>
+    <t>C     -0.47033632     4.15224075    -0.50221658</t>
+  </si>
+  <si>
+    <t>H     -1.51444888     4.07614803    -0.20615172</t>
+  </si>
+  <si>
+    <t>C     -0.13957155     4.81648254    -1.67432761</t>
+  </si>
+  <si>
+    <t>H     -0.92868316     5.23178482    -2.29559851</t>
+  </si>
+  <si>
+    <t>C      1.19329047     4.96882868    -2.05009389</t>
+  </si>
+  <si>
+    <t>H      1.45161724     5.49671555    -2.96276236</t>
+  </si>
+  <si>
+    <t>C      2.18836761     4.43753719    -1.23602724</t>
+  </si>
+  <si>
+    <t>H      3.23298573     4.55282640    -1.51245713</t>
+  </si>
+  <si>
+    <t>C      1.86140656     3.77245212    -0.06108701</t>
+  </si>
+  <si>
+    <t>H      2.65566516     3.41043568     0.58491546</t>
+  </si>
+  <si>
+    <t>N     -1.46707034     0.19585761     1.10508585</t>
+  </si>
+  <si>
+    <t>N     -0.27456889     0.29352719    -1.46418381</t>
+  </si>
+  <si>
+    <t>N      1.56698060    -0.17029783     0.71056414</t>
+  </si>
+  <si>
+    <t>O     -0.56461346    -1.56859565    -2.63991857</t>
+  </si>
+  <si>
+    <t>O     -2.41878939    -1.78692949     1.41608226</t>
+  </si>
+  <si>
+    <t>O      2.06347752    -2.33967161     0.79187685</t>
+  </si>
+  <si>
+    <t>feopt07</t>
+  </si>
+  <si>
+    <t>Fe      0.16195115     1.15102506     0.26889980</t>
+  </si>
+  <si>
+    <t>C      0.38864794     2.62661624     1.60583746</t>
+  </si>
+  <si>
+    <t>H     -0.53474694     2.93806458     2.09940839</t>
+  </si>
+  <si>
+    <t>H      1.18684053     2.50454640     2.33918428</t>
+  </si>
+  <si>
+    <t>C      0.72511816     3.46874475     0.46160641</t>
+  </si>
+  <si>
+    <t>C     -0.28722861     4.09191942    -0.30862221</t>
+  </si>
+  <si>
+    <t>H     -1.31726408     4.03187847     0.03639847</t>
+  </si>
+  <si>
+    <t>C      0.01011240     4.82837629    -1.44603419</t>
+  </si>
+  <si>
+    <t>H     -0.79220694     5.31647539    -1.99302745</t>
+  </si>
+  <si>
+    <t>C      1.32730985     4.95988369    -1.88034892</t>
+  </si>
+  <si>
+    <t>H      1.56003606     5.54392862    -2.76527691</t>
+  </si>
+  <si>
+    <t>C      2.34028435     4.33456182    -1.16061211</t>
+  </si>
+  <si>
+    <t>H      3.37337732     4.43220615    -1.48329282</t>
+  </si>
+  <si>
+    <t>C      2.04685044     3.59693217    -0.02064480</t>
+  </si>
+  <si>
+    <t>H      2.85768056     3.15993404     0.55452812</t>
+  </si>
+  <si>
+    <t>C      0.38515496     2.66331625     1.72435880</t>
+  </si>
+  <si>
+    <t>H     -0.44131351     2.80504370     2.42445731</t>
+  </si>
+  <si>
+    <t>H      1.33050644     2.59467793     2.26418066</t>
+  </si>
+  <si>
+    <t>C      0.36724114     3.63117599     0.63139844</t>
+  </si>
+  <si>
+    <t>C     -0.85274041     4.16804790     0.15196133</t>
+  </si>
+  <si>
+    <t>H     -1.77062917     3.94004726     0.68966138</t>
+  </si>
+  <si>
+    <t>C     -0.89467883     5.02565956    -0.93763518</t>
+  </si>
+  <si>
+    <t>H     -1.84729195     5.44043684    -1.25645089</t>
+  </si>
+  <si>
+    <t>C      0.27412736     5.37072849    -1.61275148</t>
+  </si>
+  <si>
+    <t>H      0.24153170     6.04909134    -2.45959258</t>
+  </si>
+  <si>
+    <t>C      1.48416162     4.83579636    -1.18282366</t>
+  </si>
+  <si>
+    <t>H      2.40535998     5.09957790    -1.69541693</t>
+  </si>
+  <si>
+    <t>C      1.53057814     3.97736168    -0.09165478</t>
+  </si>
+  <si>
+    <t>H      2.49145579     3.61198425     0.25828719</t>
+  </si>
+  <si>
+    <t>feopt08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -994,13 +1289,27 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1019,11 +1328,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1046,71 +1358,67 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="testtomfe" connectionId="13" xr16:uid="{00000000-0016-0000-0000-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tomfe_6311+g*" connectionId="13" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf04_coords" connectionId="7" xr16:uid="{0EACA580-A4B7-AE47-ADBE-D49205E98595}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf04_coords" connectionId="6" xr16:uid="{0EACA580-A4B7-AE47-ADBE-D49205E98595}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf04_s30_coords" connectionId="8" xr16:uid="{8018AD0E-E07A-364F-98CA-4224DCC4E142}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf02_631g_coor" connectionId="5" xr16:uid="{3AF8AE73-85C2-C34F-B0D5-46836E36B42A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf02_631g_coor" connectionId="6" xr16:uid="{3AF8AE73-85C2-C34F-B0D5-46836E36B42A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf05" connectionId="9" xr16:uid="{93D7A032-4C04-6549-B01E-8621DC3041B5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tomfe1-02coor" connectionId="16" xr16:uid="{00000000-0016-0000-0100-000006000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf05_1" connectionId="10" xr16:uid="{A3551B01-7EAB-8E41-A26C-C33123B0B459}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="feopt05_coords" connectionId="5" xr16:uid="{71C92314-5655-4241-92EB-012A9836F714}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tomfebn_start02" connectionId="16" xr16:uid="{00000000-0016-0000-0100-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf04_s35_coords" connectionId="8" xr16:uid="{137057B6-B9E4-3643-9B68-1FB6CFFFCF01}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fedft05_coords" connectionId="3" xr16:uid="{66F142BC-748E-2644-83A2-108843A27753}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf04_s35_coords" connectionId="9" xr16:uid="{137057B6-B9E4-3643-9B68-1FB6CFFFCF01}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="feopt05_6311g_coords" connectionId="4" xr16:uid="{5AE73355-1452-CD47-9473-BCDFBAC39503}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tomfe_6311+g*" connectionId="14" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tomfe_631g" connectionId="14" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tomfe_631g" connectionId="15" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="testtomfe" connectionId="12" xr16:uid="{00000000-0016-0000-0000-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf05_1" connectionId="11" xr16:uid="{A3551B01-7EAB-8E41-A26C-C33123B0B459}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="run1_coordinates_end" connectionId="11" xr16:uid="{00000000-0016-0000-0100-000007000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf04_s30_coords" connectionId="7" xr16:uid="{8018AD0E-E07A-364F-98CA-4224DCC4E142}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="feopt05_coords" connectionId="4" xr16:uid="{71C92314-5655-4241-92EB-012A9836F714}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="2018_1fe03_coordinates" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fescf05" connectionId="10" xr16:uid="{93D7A032-4C04-6549-B01E-8621DC3041B5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="run1_coordinates_end" connectionId="12" xr16:uid="{00000000-0016-0000-0100-000007000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tomfebn_start02" connectionId="17" xr16:uid="{00000000-0016-0000-0100-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="2018.06.15_coordinates" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="2018.06.15_coordinates" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tomfe1-02coor" connectionId="15" xr16:uid="{00000000-0016-0000-0100-000006000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4906,7 +5214,7 @@
   <dimension ref="A1:CW75"/>
   <sheetViews>
     <sheetView topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="CN1" sqref="CN1:CW74"/>
+      <selection activeCell="CT31" sqref="CT31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19736,10 +20044,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BB2B4B-904D-EA4B-B0ED-571736EDF1C2}">
-  <dimension ref="F1:U74"/>
+  <dimension ref="F1:Z74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F50" workbookViewId="0">
-      <selection activeCell="U74" sqref="R3:U74"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:Z74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19762,7 +20070,7 @@
     <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F1" t="s">
         <v>118</v>
       </c>
@@ -19772,8 +20080,14 @@
       <c r="R1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="2" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W1" t="s">
+        <v>192</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>119</v>
       </c>
@@ -19783,8 +20097,14 @@
       <c r="R2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="3" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W2" t="s">
+        <v>195</v>
+      </c>
+      <c r="X2" s="1">
+        <v>43353</v>
+      </c>
+    </row>
+    <row r="3" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F3" s="3" t="s">
         <v>120</v>
       </c>
@@ -19812,8 +20132,20 @@
       <c r="U3">
         <v>0.33111718000000001</v>
       </c>
-    </row>
-    <row r="4" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>5.3084310000000003E-2</v>
+      </c>
+      <c r="Y3">
+        <v>1.28052583</v>
+      </c>
+      <c r="Z3">
+        <v>0.3123435</v>
+      </c>
+    </row>
+    <row r="4" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F4" s="3" t="s">
         <v>121</v>
       </c>
@@ -19841,8 +20173,20 @@
       <c r="U4">
         <v>-9.7872399999999991E-3</v>
       </c>
-    </row>
-    <row r="5" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <v>-0.30543609999999999</v>
+      </c>
+      <c r="Y4">
+        <v>-1.82500453</v>
+      </c>
+      <c r="Z4">
+        <v>-4.7288749999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F5" s="3" t="s">
         <v>122</v>
       </c>
@@ -19870,8 +20214,20 @@
       <c r="U5">
         <v>3.4642392200000001</v>
       </c>
-    </row>
-    <row r="6" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>-2.0298163699999998</v>
+      </c>
+      <c r="Y5">
+        <v>0.69045992</v>
+      </c>
+      <c r="Z5">
+        <v>3.4482965800000001</v>
+      </c>
+    </row>
+    <row r="6" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F6" s="3" t="s">
         <v>123</v>
       </c>
@@ -19899,8 +20255,20 @@
       <c r="U6">
         <v>3.8046582899999999</v>
       </c>
-    </row>
-    <row r="7" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X6">
+        <v>-1.4932832899999999</v>
+      </c>
+      <c r="Y6">
+        <v>-0.19829063999999999</v>
+      </c>
+      <c r="Z6">
+        <v>3.7933076400000001</v>
+      </c>
+    </row>
+    <row r="7" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F7" s="3" t="s">
         <v>124</v>
       </c>
@@ -19928,8 +20296,20 @@
       <c r="U7">
         <v>4.1727717599999998</v>
       </c>
-    </row>
-    <row r="8" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7">
+        <v>-2.84520843</v>
+      </c>
+      <c r="Y7">
+        <v>0.89073910000000001</v>
+      </c>
+      <c r="Z7">
+        <v>4.1514751099999998</v>
+      </c>
+    </row>
+    <row r="8" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F8" s="3" t="s">
         <v>125</v>
       </c>
@@ -19957,8 +20337,20 @@
       <c r="U8">
         <v>3.4612863599999999</v>
       </c>
-    </row>
-    <row r="9" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W8" t="s">
+        <v>4</v>
+      </c>
+      <c r="X8">
+        <v>-1.3366315499999999</v>
+      </c>
+      <c r="Y8">
+        <v>1.53179983</v>
+      </c>
+      <c r="Z8">
+        <v>3.4752312000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F9" s="3" t="s">
         <v>126</v>
       </c>
@@ -19986,8 +20378,20 @@
       <c r="U9">
         <v>2.0651367999999999</v>
       </c>
-    </row>
-    <row r="10" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W9" t="s">
+        <v>3</v>
+      </c>
+      <c r="X9">
+        <v>-2.5802639900000002</v>
+      </c>
+      <c r="Y9">
+        <v>0.47248098999999999</v>
+      </c>
+      <c r="Z9">
+        <v>2.0401646000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F10" s="3" t="s">
         <v>127</v>
       </c>
@@ -20015,8 +20419,20 @@
       <c r="U10">
         <v>1.5760252100000001</v>
       </c>
-    </row>
-    <row r="11" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W10" t="s">
+        <v>3</v>
+      </c>
+      <c r="X10">
+        <v>-3.41571772</v>
+      </c>
+      <c r="Y10">
+        <v>1.6556706999999999</v>
+      </c>
+      <c r="Z10">
+        <v>1.5785370299999999</v>
+      </c>
+    </row>
+    <row r="11" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F11" s="3" t="s">
         <v>128</v>
       </c>
@@ -20044,8 +20460,20 @@
       <c r="U11">
         <v>1.59802413</v>
       </c>
-    </row>
-    <row r="12" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W11" t="s">
+        <v>4</v>
+      </c>
+      <c r="X11">
+        <v>-2.8408813999999998</v>
+      </c>
+      <c r="Y11">
+        <v>2.5834136999999999</v>
+      </c>
+      <c r="Z11">
+        <v>1.62685641</v>
+      </c>
+    </row>
+    <row r="12" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F12" s="3" t="s">
         <v>129</v>
       </c>
@@ -20073,8 +20501,20 @@
       <c r="U12">
         <v>2.2128485800000002</v>
       </c>
-    </row>
-    <row r="13" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W12" t="s">
+        <v>4</v>
+      </c>
+      <c r="X12">
+        <v>-4.2984314000000001</v>
+      </c>
+      <c r="Y12">
+        <v>1.77881355</v>
+      </c>
+      <c r="Z12">
+        <v>2.2144044100000002</v>
+      </c>
+    </row>
+    <row r="13" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F13" s="3" t="s">
         <v>130</v>
       </c>
@@ -20102,8 +20542,20 @@
       <c r="U13">
         <v>0.55226189000000003</v>
       </c>
-    </row>
-    <row r="14" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W13" t="s">
+        <v>4</v>
+      </c>
+      <c r="X13">
+        <v>-3.7534316200000002</v>
+      </c>
+      <c r="Y13">
+        <v>1.5153502400000001</v>
+      </c>
+      <c r="Z13">
+        <v>0.54797812999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F14" s="3" t="s">
         <v>131</v>
       </c>
@@ -20131,8 +20583,20 @@
       <c r="U14">
         <v>2.0111413599999999</v>
       </c>
-    </row>
-    <row r="15" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W14" t="s">
+        <v>3</v>
+      </c>
+      <c r="X14">
+        <v>-3.3582180899999998</v>
+      </c>
+      <c r="Y14">
+        <v>-0.84951829999999995</v>
+      </c>
+      <c r="Z14">
+        <v>1.9587014700000001</v>
+      </c>
+    </row>
+    <row r="15" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F15" s="3" t="s">
         <v>132</v>
       </c>
@@ -20160,8 +20624,20 @@
       <c r="U15">
         <v>2.9846720800000002</v>
       </c>
-    </row>
-    <row r="16" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W15" t="s">
+        <v>4</v>
+      </c>
+      <c r="X15">
+        <v>-3.6969055900000001</v>
+      </c>
+      <c r="Y15">
+        <v>-1.22527271</v>
+      </c>
+      <c r="Z15">
+        <v>2.9254328200000002</v>
+      </c>
+    </row>
+    <row r="16" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F16" s="3" t="s">
         <v>133</v>
       </c>
@@ -20189,8 +20665,20 @@
       <c r="U16">
         <v>1.3238987900000001</v>
       </c>
-    </row>
-    <row r="17" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W16" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16">
+        <v>-4.2102951400000004</v>
+      </c>
+      <c r="Y16">
+        <v>-0.79377538999999997</v>
+      </c>
+      <c r="Z16">
+        <v>1.27204333</v>
+      </c>
+    </row>
+    <row r="17" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F17" s="3" t="s">
         <v>134</v>
       </c>
@@ -20218,8 +20706,20 @@
       <c r="U17">
         <v>0.89301227999999999</v>
       </c>
-    </row>
-    <row r="18" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W17" t="s">
+        <v>3</v>
+      </c>
+      <c r="X17">
+        <v>-1.42430766</v>
+      </c>
+      <c r="Y17">
+        <v>-1.0717599499999999</v>
+      </c>
+      <c r="Z17">
+        <v>0.86894534999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F18" s="3" t="s">
         <v>135</v>
       </c>
@@ -20247,8 +20747,20 @@
       <c r="U18">
         <v>-3.1960113899999998</v>
       </c>
-    </row>
-    <row r="19" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W18" t="s">
+        <v>3</v>
+      </c>
+      <c r="X18">
+        <v>0.84463270000000001</v>
+      </c>
+      <c r="Y18">
+        <v>1.5645013699999999</v>
+      </c>
+      <c r="Z18">
+        <v>-3.2536082999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F19" s="3" t="s">
         <v>136</v>
       </c>
@@ -20276,8 +20788,20 @@
       <c r="U19">
         <v>-2.5619415399999999</v>
       </c>
-    </row>
-    <row r="20" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W19" t="s">
+        <v>4</v>
+      </c>
+      <c r="X19">
+        <v>0.95358721000000002</v>
+      </c>
+      <c r="Y19">
+        <v>2.4716466600000002</v>
+      </c>
+      <c r="Z19">
+        <v>-2.6548383800000002</v>
+      </c>
+    </row>
+    <row r="20" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F20" s="3" t="s">
         <v>137</v>
       </c>
@@ -20305,8 +20829,20 @@
       <c r="U20">
         <v>-4.2353814999999999</v>
       </c>
-    </row>
-    <row r="21" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W20" t="s">
+        <v>4</v>
+      </c>
+      <c r="X20">
+        <v>0.78632484999999996</v>
+      </c>
+      <c r="Y20">
+        <v>1.86287881</v>
+      </c>
+      <c r="Z20">
+        <v>-4.3057477000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F21" s="3" t="s">
         <v>138</v>
       </c>
@@ -20334,8 +20870,20 @@
       <c r="U21">
         <v>-3.0790366200000001</v>
       </c>
-    </row>
-    <row r="22" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W21" t="s">
+        <v>4</v>
+      </c>
+      <c r="X21">
+        <v>1.7434746699999999</v>
+      </c>
+      <c r="Y21">
+        <v>0.95600417000000004</v>
+      </c>
+      <c r="Z21">
+        <v>-3.1204059700000002</v>
+      </c>
+    </row>
+    <row r="22" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F22" s="3" t="s">
         <v>139</v>
       </c>
@@ -20363,8 +20911,20 @@
       <c r="U22">
         <v>-2.82152577</v>
       </c>
-    </row>
-    <row r="23" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W22" t="s">
+        <v>3</v>
+      </c>
+      <c r="X22">
+        <v>-0.3989393</v>
+      </c>
+      <c r="Y22">
+        <v>0.78359533999999997</v>
+      </c>
+      <c r="Z22">
+        <v>-2.8507298599999999</v>
+      </c>
+    </row>
+    <row r="23" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F23" s="3" t="s">
         <v>140</v>
       </c>
@@ -20392,8 +20952,20 @@
       <c r="U23">
         <v>-2.9211008299999999</v>
       </c>
-    </row>
-    <row r="24" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W23" t="s">
+        <v>3</v>
+      </c>
+      <c r="X23">
+        <v>-1.6521990200000001</v>
+      </c>
+      <c r="Y23">
+        <v>1.6426283800000001</v>
+      </c>
+      <c r="Z23">
+        <v>-2.9855547800000002</v>
+      </c>
+    </row>
+    <row r="24" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F24" s="3" t="s">
         <v>141</v>
       </c>
@@ -20421,8 +20993,20 @@
       <c r="U24">
         <v>-2.6384221499999998</v>
       </c>
-    </row>
-    <row r="25" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W24" t="s">
+        <v>4</v>
+      </c>
+      <c r="X24">
+        <v>-2.5411950499999998</v>
+      </c>
+      <c r="Y24">
+        <v>1.0822184699999999</v>
+      </c>
+      <c r="Z24">
+        <v>-2.6820371999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F25" s="3" t="s">
         <v>142</v>
       </c>
@@ -20450,8 +21034,20 @@
       <c r="U25">
         <v>-3.9434456899999999</v>
       </c>
-    </row>
-    <row r="26" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W25" t="s">
+        <v>4</v>
+      </c>
+      <c r="X25">
+        <v>-1.78834589</v>
+      </c>
+      <c r="Y25">
+        <v>1.96629846</v>
+      </c>
+      <c r="Z25">
+        <v>-4.02274362</v>
+      </c>
+    </row>
+    <row r="26" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F26" s="3" t="s">
         <v>143</v>
       </c>
@@ -20479,8 +21075,20 @@
       <c r="U26">
         <v>-2.2585922799999998</v>
       </c>
-    </row>
-    <row r="27" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W26" t="s">
+        <v>4</v>
+      </c>
+      <c r="X26">
+        <v>-1.57746699</v>
+      </c>
+      <c r="Y26">
+        <v>2.53641278</v>
+      </c>
+      <c r="Z26">
+        <v>-2.36117446</v>
+      </c>
+    </row>
+    <row r="27" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F27" s="3" t="s">
         <v>144</v>
       </c>
@@ -20508,8 +21116,20 @@
       <c r="U27">
         <v>-3.64185596</v>
       </c>
-    </row>
-    <row r="28" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W27" t="s">
+        <v>3</v>
+      </c>
+      <c r="X27">
+        <v>-0.52638600999999996</v>
+      </c>
+      <c r="Y27">
+        <v>-0.53760218999999998</v>
+      </c>
+      <c r="Z27">
+        <v>-3.6369934599999998</v>
+      </c>
+    </row>
+    <row r="28" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F28" s="3" t="s">
         <v>145</v>
       </c>
@@ -20537,8 +21157,20 @@
       <c r="U28">
         <v>-4.2268117900000002</v>
       </c>
-    </row>
-    <row r="29" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W28" t="s">
+        <v>4</v>
+      </c>
+      <c r="X28">
+        <v>-1.4432126700000001</v>
+      </c>
+      <c r="Y28">
+        <v>-0.60385568000000001</v>
+      </c>
+      <c r="Z28">
+        <v>-4.2275911400000004</v>
+      </c>
+    </row>
+    <row r="29" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F29" s="3" t="s">
         <v>146</v>
       </c>
@@ -20566,8 +21198,20 @@
       <c r="U29">
         <v>-4.27928804</v>
       </c>
-    </row>
-    <row r="30" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X29">
+        <v>0.33189657</v>
+      </c>
+      <c r="Y29">
+        <v>-0.73049620000000004</v>
+      </c>
+      <c r="Z29">
+        <v>-4.2866518200000003</v>
+      </c>
+    </row>
+    <row r="30" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F30" s="3" t="s">
         <v>147</v>
       </c>
@@ -20595,8 +21239,20 @@
       <c r="U30">
         <v>-1.3990002100000001</v>
       </c>
-    </row>
-    <row r="31" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W30" t="s">
+        <v>3</v>
+      </c>
+      <c r="X30">
+        <v>-0.3886096</v>
+      </c>
+      <c r="Y30">
+        <v>-0.98677168999999998</v>
+      </c>
+      <c r="Z30">
+        <v>-1.4408494599999999</v>
+      </c>
+    </row>
+    <row r="31" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F31" s="3" t="s">
         <v>148</v>
       </c>
@@ -20624,8 +21280,20 @@
       <c r="U31">
         <v>2.3331226200000001</v>
       </c>
-    </row>
-    <row r="32" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W31" t="s">
+        <v>3</v>
+      </c>
+      <c r="X31">
+        <v>3.2937205899999999</v>
+      </c>
+      <c r="Y31">
+        <v>0.63657680999999999</v>
+      </c>
+      <c r="Z31">
+        <v>2.3144055699999999</v>
+      </c>
+    </row>
+    <row r="32" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F32" s="3" t="s">
         <v>149</v>
       </c>
@@ -20653,8 +21321,20 @@
       <c r="U32">
         <v>2.11724801</v>
       </c>
-    </row>
-    <row r="33" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W32" t="s">
+        <v>4</v>
+      </c>
+      <c r="X32">
+        <v>3.1575887100000002</v>
+      </c>
+      <c r="Y32">
+        <v>1.70162334</v>
+      </c>
+      <c r="Z32">
+        <v>2.1194169999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F33" s="3" t="s">
         <v>150</v>
       </c>
@@ -20682,8 +21362,20 @@
       <c r="U33">
         <v>2.6640509899999998</v>
       </c>
-    </row>
-    <row r="34" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W33" t="s">
+        <v>4</v>
+      </c>
+      <c r="X33">
+        <v>4.3298833999999999</v>
+      </c>
+      <c r="Y33">
+        <v>0.48817368999999999</v>
+      </c>
+      <c r="Z33">
+        <v>2.6363900600000001</v>
+      </c>
+    </row>
+    <row r="34" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F34" s="3" t="s">
         <v>151</v>
       </c>
@@ -20711,8 +21403,20 @@
       <c r="U34">
         <v>3.14950383</v>
       </c>
-    </row>
-    <row r="35" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W34" t="s">
+        <v>4</v>
+      </c>
+      <c r="X34">
+        <v>2.6346573100000001</v>
+      </c>
+      <c r="Y34">
+        <v>0.35726848999999999</v>
+      </c>
+      <c r="Z34">
+        <v>3.14056202</v>
+      </c>
+    </row>
+    <row r="35" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F35" s="3" t="s">
         <v>152</v>
       </c>
@@ -20740,8 +21444,20 @@
       <c r="U35">
         <v>1.10471875</v>
       </c>
-    </row>
-    <row r="36" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W35" t="s">
+        <v>3</v>
+      </c>
+      <c r="X35">
+        <v>2.9983885199999998</v>
+      </c>
+      <c r="Y35">
+        <v>-0.20076206999999999</v>
+      </c>
+      <c r="Z35">
+        <v>1.0792377099999999</v>
+      </c>
+    </row>
+    <row r="36" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F36" s="3" t="s">
         <v>153</v>
       </c>
@@ -20769,8 +21485,20 @@
       <c r="U36">
         <v>-0.10341662</v>
       </c>
-    </row>
-    <row r="37" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W36" t="s">
+        <v>3</v>
+      </c>
+      <c r="X36">
+        <v>3.82464103</v>
+      </c>
+      <c r="Y36">
+        <v>0.26684225</v>
+      </c>
+      <c r="Z36">
+        <v>-0.1171201</v>
+      </c>
+    </row>
+    <row r="37" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F37" s="3" t="s">
         <v>154</v>
       </c>
@@ -20798,8 +21526,20 @@
       <c r="U37">
         <v>-0.94534448999999998</v>
       </c>
-    </row>
-    <row r="38" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W37" t="s">
+        <v>4</v>
+      </c>
+      <c r="X37">
+        <v>3.6718260300000001</v>
+      </c>
+      <c r="Y37">
+        <v>-0.39571588000000002</v>
+      </c>
+      <c r="Z37">
+        <v>-0.97414729</v>
+      </c>
+    </row>
+    <row r="38" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F38" s="3" t="s">
         <v>155</v>
       </c>
@@ -20827,8 +21567,20 @@
       <c r="U38">
         <v>0.13656429</v>
       </c>
-    </row>
-    <row r="39" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W38" t="s">
+        <v>4</v>
+      </c>
+      <c r="X38">
+        <v>4.8928892299999998</v>
+      </c>
+      <c r="Y38">
+        <v>0.27347111000000002</v>
+      </c>
+      <c r="Z38">
+        <v>0.12424092</v>
+      </c>
+    </row>
+    <row r="39" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F39" s="3" t="s">
         <v>156</v>
       </c>
@@ -20856,8 +21608,20 @@
       <c r="U39">
         <v>-0.41218272</v>
       </c>
-    </row>
-    <row r="40" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W39" t="s">
+        <v>4</v>
+      </c>
+      <c r="X39">
+        <v>3.5335902199999998</v>
+      </c>
+      <c r="Y39">
+        <v>1.27579295</v>
+      </c>
+      <c r="Z39">
+        <v>-0.41912891000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F40" s="3" t="s">
         <v>157</v>
       </c>
@@ -20885,8 +21649,20 @@
       <c r="U40">
         <v>1.4028753599999999</v>
       </c>
-    </row>
-    <row r="41" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W40" t="s">
+        <v>3</v>
+      </c>
+      <c r="X40">
+        <v>3.2125176099999999</v>
+      </c>
+      <c r="Y40">
+        <v>-1.69851982</v>
+      </c>
+      <c r="Z40">
+        <v>1.3561398499999999</v>
+      </c>
+    </row>
+    <row r="41" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F41" s="3" t="s">
         <v>158</v>
       </c>
@@ -20914,8 +21690,20 @@
       <c r="U41">
         <v>0.90155660000000004</v>
       </c>
-    </row>
-    <row r="42" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W41" t="s">
+        <v>4</v>
+      </c>
+      <c r="X41">
+        <v>4.1043784600000004</v>
+      </c>
+      <c r="Y41">
+        <v>-2.1141078000000002</v>
+      </c>
+      <c r="Z41">
+        <v>0.88339460999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F42" s="3" t="s">
         <v>159</v>
       </c>
@@ -20943,8 +21731,20 @@
       <c r="U42">
         <v>2.4717917699999998</v>
       </c>
-    </row>
-    <row r="43" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W42" t="s">
+        <v>4</v>
+      </c>
+      <c r="X42">
+        <v>3.2336552900000002</v>
+      </c>
+      <c r="Y42">
+        <v>-1.9278925600000001</v>
+      </c>
+      <c r="Z42">
+        <v>2.4270357699999998</v>
+      </c>
+    </row>
+    <row r="43" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F43" s="3" t="s">
         <v>160</v>
       </c>
@@ -20972,8 +21772,20 @@
       <c r="U43">
         <v>0.56941008000000004</v>
       </c>
-    </row>
-    <row r="44" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W43" t="s">
+        <v>3</v>
+      </c>
+      <c r="X43">
+        <v>1.1590300200000001</v>
+      </c>
+      <c r="Y43">
+        <v>-1.3802196200000001</v>
+      </c>
+      <c r="Z43">
+        <v>0.53258587999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F44" s="3" t="s">
         <v>161</v>
       </c>
@@ -21001,8 +21813,20 @@
       <c r="U44">
         <v>-3.1941539999999997E-2</v>
       </c>
-    </row>
-    <row r="45" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W44" t="s">
+        <v>3</v>
+      </c>
+      <c r="X44">
+        <v>-0.51999039999999996</v>
+      </c>
+      <c r="Y44">
+        <v>-3.4218376300000002</v>
+      </c>
+      <c r="Z44">
+        <v>-6.233851E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F45" s="3" t="s">
         <v>162</v>
       </c>
@@ -21030,8 +21854,20 @@
       <c r="U45">
         <v>-1.1704760999999999</v>
       </c>
-    </row>
-    <row r="46" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W45" t="s">
+        <v>3</v>
+      </c>
+      <c r="X45">
+        <v>-0.89046018000000005</v>
+      </c>
+      <c r="Y45">
+        <v>-4.1741158699999996</v>
+      </c>
+      <c r="Z45">
+        <v>-1.1826825599999999</v>
+      </c>
+    </row>
+    <row r="46" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F46" s="3" t="s">
         <v>163</v>
       </c>
@@ -21059,8 +21895,20 @@
       <c r="U46">
         <v>-2.1119644200000001</v>
       </c>
-    </row>
-    <row r="47" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W46" t="s">
+        <v>4</v>
+      </c>
+      <c r="X46">
+        <v>-1.02570988</v>
+      </c>
+      <c r="Y46">
+        <v>-3.68213517</v>
+      </c>
+      <c r="Z46">
+        <v>-2.1386323900000002</v>
+      </c>
+    </row>
+    <row r="47" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F47" s="3" t="s">
         <v>164</v>
       </c>
@@ -21088,8 +21936,20 @@
       <c r="U47">
         <v>-1.11739254</v>
       </c>
-    </row>
-    <row r="48" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W47" t="s">
+        <v>3</v>
+      </c>
+      <c r="X47">
+        <v>-1.08971493</v>
+      </c>
+      <c r="Y47">
+        <v>-5.5516549199999998</v>
+      </c>
+      <c r="Z47">
+        <v>-1.11062255</v>
+      </c>
+    </row>
+    <row r="48" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F48" s="3" t="s">
         <v>165</v>
       </c>
@@ -21117,8 +21977,20 @@
       <c r="U48">
         <v>-2.0163097799999998</v>
       </c>
-    </row>
-    <row r="49" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W48" t="s">
+        <v>4</v>
+      </c>
+      <c r="X48">
+        <v>-1.37601489</v>
+      </c>
+      <c r="Y48">
+        <v>-6.09995098</v>
+      </c>
+      <c r="Z48">
+        <v>-2.0048662300000002</v>
+      </c>
+    </row>
+    <row r="49" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F49" s="3" t="s">
         <v>166</v>
       </c>
@@ -21146,8 +22018,20 @@
       <c r="U49">
         <v>7.9591460000000003E-2</v>
       </c>
-    </row>
-    <row r="50" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W49" t="s">
+        <v>3</v>
+      </c>
+      <c r="X49">
+        <v>-0.9261568</v>
+      </c>
+      <c r="Y49">
+        <v>-6.2236605599999999</v>
+      </c>
+      <c r="Z49">
+        <v>9.2842430000000004E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F50" s="3" t="s">
         <v>167</v>
       </c>
@@ -21175,8 +22059,20 @@
       <c r="U50">
         <v>0.12130555</v>
       </c>
-    </row>
-    <row r="51" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W50" t="s">
+        <v>4</v>
+      </c>
+      <c r="X50">
+        <v>-1.08049076</v>
+      </c>
+      <c r="Y50">
+        <v>-7.2978599700000002</v>
+      </c>
+      <c r="Z50">
+        <v>0.15070475999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F51" s="3" t="s">
         <v>168</v>
       </c>
@@ -21204,8 +22100,20 @@
       <c r="U51">
         <v>1.22593332</v>
       </c>
-    </row>
-    <row r="52" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W51" t="s">
+        <v>3</v>
+      </c>
+      <c r="X51">
+        <v>-0.56161804000000004</v>
+      </c>
+      <c r="Y51">
+        <v>-5.5010464900000002</v>
+      </c>
+      <c r="Z51">
+        <v>1.2248054399999999</v>
+      </c>
+    </row>
+    <row r="52" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F52" s="3" t="s">
         <v>169</v>
       </c>
@@ -21233,8 +22141,20 @@
       <c r="U52">
         <v>2.1656726599999998</v>
       </c>
-    </row>
-    <row r="53" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X52">
+        <v>-0.43036148000000002</v>
+      </c>
+      <c r="Y52">
+        <v>-6.0094153700000001</v>
+      </c>
+      <c r="Z52">
+        <v>2.1768264400000001</v>
+      </c>
+    </row>
+    <row r="53" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F53" s="3" t="s">
         <v>170</v>
       </c>
@@ -21262,8 +22182,20 @@
       <c r="U53">
         <v>1.16460345</v>
       </c>
-    </row>
-    <row r="54" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W53" t="s">
+        <v>3</v>
+      </c>
+      <c r="X53">
+        <v>-0.36559821999999997</v>
+      </c>
+      <c r="Y53">
+        <v>-4.1291235100000003</v>
+      </c>
+      <c r="Z53">
+        <v>1.1395707500000001</v>
+      </c>
+    </row>
+    <row r="54" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F54" s="3" t="s">
         <v>171</v>
       </c>
@@ -21291,8 +22223,20 @@
       <c r="U54">
         <v>2.0677230400000002</v>
       </c>
-    </row>
-    <row r="55" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W54" t="s">
+        <v>4</v>
+      </c>
+      <c r="X54">
+        <v>-8.1234150000000005E-2</v>
+      </c>
+      <c r="Y54">
+        <v>-3.5922666099999998</v>
+      </c>
+      <c r="Z54">
+        <v>2.04220259</v>
+      </c>
+    </row>
+    <row r="55" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F55" s="3" t="s">
         <v>172</v>
       </c>
@@ -21320,8 +22264,20 @@
       <c r="U55">
         <v>1.6299794400000001</v>
       </c>
-    </row>
-    <row r="56" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W55" t="s">
+        <v>3</v>
+      </c>
+      <c r="X55">
+        <v>0.27978106000000003</v>
+      </c>
+      <c r="Y55">
+        <v>2.7561179099999999</v>
+      </c>
+      <c r="Z55">
+        <v>1.6492811199999999</v>
+      </c>
+    </row>
+    <row r="56" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F56" s="3" t="s">
         <v>173</v>
       </c>
@@ -21349,8 +22305,20 @@
       <c r="U56">
         <v>2.1217514400000002</v>
       </c>
-    </row>
-    <row r="57" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X56">
+        <v>-0.64361374999999998</v>
+      </c>
+      <c r="Y56">
+        <v>3.0675661600000002</v>
+      </c>
+      <c r="Z56">
+        <v>2.1428520600000001</v>
+      </c>
+    </row>
+    <row r="57" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F57" s="3" t="s">
         <v>174</v>
       </c>
@@ -21378,8 +22346,20 @@
       <c r="U57">
         <v>2.3650597000000002</v>
       </c>
-    </row>
-    <row r="58" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W57" t="s">
+        <v>4</v>
+      </c>
+      <c r="X57">
+        <v>1.07797371</v>
+      </c>
+      <c r="Y57">
+        <v>2.6340478699999998</v>
+      </c>
+      <c r="Z57">
+        <v>2.38262792</v>
+      </c>
+    </row>
+    <row r="58" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F58" s="3" t="s">
         <v>175</v>
       </c>
@@ -21407,8 +22387,20 @@
       <c r="U58">
         <v>0.49093331000000001</v>
       </c>
-    </row>
-    <row r="59" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W58" t="s">
+        <v>3</v>
+      </c>
+      <c r="X58">
+        <v>0.61625132000000005</v>
+      </c>
+      <c r="Y58">
+        <v>3.5982463999999998</v>
+      </c>
+      <c r="Z58">
+        <v>0.50504998999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F59" s="3" t="s">
         <v>176</v>
       </c>
@@ -21436,8 +22428,20 @@
       <c r="U59">
         <v>-0.26536929999999997</v>
       </c>
-    </row>
-    <row r="60" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W59" t="s">
+        <v>3</v>
+      </c>
+      <c r="X59">
+        <v>-0.39609545000000002</v>
+      </c>
+      <c r="Y59">
+        <v>4.2214214500000002</v>
+      </c>
+      <c r="Z59">
+        <v>-0.26517851999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F60" s="3" t="s">
         <v>177</v>
       </c>
@@ -21465,8 +22469,20 @@
       <c r="U60">
         <v>8.1946699999999997E-2</v>
       </c>
-    </row>
-    <row r="61" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W60" t="s">
+        <v>4</v>
+      </c>
+      <c r="X60">
+        <v>-1.42613089</v>
+      </c>
+      <c r="Y60">
+        <v>4.1613802499999997</v>
+      </c>
+      <c r="Z60">
+        <v>7.9842129999999997E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F61" s="3" t="s">
         <v>178</v>
       </c>
@@ -21494,8 +22510,20 @@
       <c r="U61">
         <v>-1.3954099200000001</v>
       </c>
-    </row>
-    <row r="62" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W61" t="s">
+        <v>3</v>
+      </c>
+      <c r="X61">
+        <v>-9.8754400000000006E-2</v>
+      </c>
+      <c r="Y61">
+        <v>4.9578781200000002</v>
+      </c>
+      <c r="Z61">
+        <v>-1.4025905599999999</v>
+      </c>
+    </row>
+    <row r="62" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F62" s="3" t="s">
         <v>179</v>
       </c>
@@ -21523,8 +22551,20 @@
       <c r="U62">
         <v>-1.9334553699999999</v>
       </c>
-    </row>
-    <row r="63" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W62" t="s">
+        <v>4</v>
+      </c>
+      <c r="X62">
+        <v>-0.90107378000000005</v>
+      </c>
+      <c r="Y62">
+        <v>5.4459774400000001</v>
+      </c>
+      <c r="Z62">
+        <v>-1.9495838000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F63" s="3" t="s">
         <v>180</v>
       </c>
@@ -21552,8 +22592,20 @@
       <c r="U63">
         <v>-1.8301770399999999</v>
       </c>
-    </row>
-    <row r="64" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W63" t="s">
+        <v>3</v>
+      </c>
+      <c r="X63">
+        <v>1.2184429800000001</v>
+      </c>
+      <c r="Y63">
+        <v>5.0893853699999996</v>
+      </c>
+      <c r="Z63">
+        <v>-1.8369052699999999</v>
+      </c>
+    </row>
+    <row r="64" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F64" s="3" t="s">
         <v>181</v>
       </c>
@@ -21581,8 +22633,20 @@
       <c r="U64">
         <v>-2.7040490199999998</v>
       </c>
-    </row>
-    <row r="65" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W64" t="s">
+        <v>4</v>
+      </c>
+      <c r="X64">
+        <v>1.45116925</v>
+      </c>
+      <c r="Y64">
+        <v>5.6734304299999998</v>
+      </c>
+      <c r="Z64">
+        <v>-2.7218331199999999</v>
+      </c>
+    </row>
+    <row r="65" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F65" s="3" t="s">
         <v>182</v>
       </c>
@@ -21610,8 +22674,20 @@
       <c r="U65">
         <v>-1.11545523</v>
       </c>
-    </row>
-    <row r="66" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W65" t="s">
+        <v>3</v>
+      </c>
+      <c r="X65">
+        <v>2.23141743</v>
+      </c>
+      <c r="Y65">
+        <v>4.4640636599999999</v>
+      </c>
+      <c r="Z65">
+        <v>-1.1171684</v>
+      </c>
+    </row>
+    <row r="66" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F66" s="3" t="s">
         <v>183</v>
       </c>
@@ -21639,8 +22715,20 @@
       <c r="U66">
         <v>-1.43428723</v>
       </c>
-    </row>
-    <row r="67" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W66" t="s">
+        <v>4</v>
+      </c>
+      <c r="X66">
+        <v>3.2645103799999999</v>
+      </c>
+      <c r="Y66">
+        <v>4.5617077699999999</v>
+      </c>
+      <c r="Z66">
+        <v>-1.4398491499999999</v>
+      </c>
+    </row>
+    <row r="67" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F67" s="3" t="s">
         <v>184</v>
       </c>
@@ -21668,8 +22756,20 @@
       <c r="U67">
         <v>1.713953E-2</v>
       </c>
-    </row>
-    <row r="68" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W67" t="s">
+        <v>3</v>
+      </c>
+      <c r="X67">
+        <v>1.9379836800000001</v>
+      </c>
+      <c r="Y67">
+        <v>3.7264337799999998</v>
+      </c>
+      <c r="Z67">
+        <v>2.2798840000000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F68" s="3" t="s">
         <v>185</v>
       </c>
@@ -21697,8 +22797,20 @@
       <c r="U68">
         <v>0.58564311999999996</v>
       </c>
-    </row>
-    <row r="69" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W68" t="s">
+        <v>4</v>
+      </c>
+      <c r="X68">
+        <v>2.7488137199999998</v>
+      </c>
+      <c r="Y68">
+        <v>3.28943553</v>
+      </c>
+      <c r="Z68">
+        <v>0.59797171000000005</v>
+      </c>
+    </row>
+    <row r="69" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F69" s="3" t="s">
         <v>186</v>
       </c>
@@ -21726,8 +22838,20 @@
       <c r="U69">
         <v>1.1195222199999999</v>
       </c>
-    </row>
-    <row r="70" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W69" t="s">
+        <v>2</v>
+      </c>
+      <c r="X69">
+        <v>-1.4670704000000001</v>
+      </c>
+      <c r="Y69">
+        <v>0.19585760999999999</v>
+      </c>
+      <c r="Z69">
+        <v>1.1050858699999999</v>
+      </c>
+    </row>
+    <row r="70" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F70" s="3" t="s">
         <v>187</v>
       </c>
@@ -21755,8 +22879,20 @@
       <c r="U70">
         <v>-1.42485704</v>
       </c>
-    </row>
-    <row r="71" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W70" t="s">
+        <v>2</v>
+      </c>
+      <c r="X70">
+        <v>-0.27456888000000002</v>
+      </c>
+      <c r="Y70">
+        <v>0.29352719999999999</v>
+      </c>
+      <c r="Z70">
+        <v>-1.46418381</v>
+      </c>
+    </row>
+    <row r="71" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F71" s="3" t="s">
         <v>188</v>
       </c>
@@ -21784,8 +22920,20 @@
       <c r="U71">
         <v>0.72373330000000002</v>
       </c>
-    </row>
-    <row r="72" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W71" t="s">
+        <v>2</v>
+      </c>
+      <c r="X71">
+        <v>1.56698062</v>
+      </c>
+      <c r="Y71">
+        <v>-0.17029783000000001</v>
+      </c>
+      <c r="Z71">
+        <v>0.71056412000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F72" s="3" t="s">
         <v>189</v>
       </c>
@@ -21813,8 +22961,20 @@
       <c r="U72">
         <v>-2.6383065700000001</v>
       </c>
-    </row>
-    <row r="73" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W72" t="s">
+        <v>1</v>
+      </c>
+      <c r="X72">
+        <v>-0.56461344000000002</v>
+      </c>
+      <c r="Y72">
+        <v>-1.5685956700000001</v>
+      </c>
+      <c r="Z72">
+        <v>-2.6399185699999999</v>
+      </c>
+    </row>
+    <row r="73" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F73" s="3" t="s">
         <v>190</v>
       </c>
@@ -21842,8 +23002,20 @@
       <c r="U73">
         <v>1.4663783699999999</v>
       </c>
-    </row>
-    <row r="74" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="W73" t="s">
+        <v>1</v>
+      </c>
+      <c r="X73">
+        <v>-2.41878927</v>
+      </c>
+      <c r="Y73">
+        <v>-1.78692951</v>
+      </c>
+      <c r="Z73">
+        <v>1.4160822900000001</v>
+      </c>
+    </row>
+    <row r="74" spans="6:26" x14ac:dyDescent="0.2">
       <c r="F74" s="3" t="s">
         <v>191</v>
       </c>
@@ -21873,6 +23045,18 @@
       </c>
       <c r="U74">
         <v>0.86590829000000002</v>
+      </c>
+      <c r="W74" t="s">
+        <v>1</v>
+      </c>
+      <c r="X74">
+        <v>2.0634775799999998</v>
+      </c>
+      <c r="Y74">
+        <v>-2.33967167</v>
+      </c>
+      <c r="Z74">
+        <v>0.79187686999999995</v>
       </c>
     </row>
   </sheetData>
@@ -21881,23 +23065,1849 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37858B7D-257D-454A-8929-F0E5BB68B834}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938D6A16-BFE4-1E47-95F0-AD738167E67D}">
+  <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K1" t="s">
+        <v>270</v>
+      </c>
+      <c r="P1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43353</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43375</v>
+      </c>
+      <c r="K2" s="1">
+        <v>43376</v>
+      </c>
+      <c r="P2" s="1">
+        <v>43376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>5.3084310000000003E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.28052583</v>
+      </c>
+      <c r="D3">
+        <v>0.3123435</v>
+      </c>
+      <c r="F3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="P3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>-0.30543609999999999</v>
+      </c>
+      <c r="C4">
+        <v>-1.82500453</v>
+      </c>
+      <c r="D4">
+        <v>-4.7288749999999997E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>199</v>
+      </c>
+      <c r="K4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>-2.0298163699999998</v>
+      </c>
+      <c r="C5">
+        <v>0.69045992</v>
+      </c>
+      <c r="D5">
+        <v>3.4482965800000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>200</v>
+      </c>
+      <c r="K5" t="s">
+        <v>200</v>
+      </c>
+      <c r="P5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>-1.4932832899999999</v>
+      </c>
+      <c r="C6">
+        <v>-0.19829063999999999</v>
+      </c>
+      <c r="D6">
+        <v>3.7933076400000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K6" t="s">
+        <v>201</v>
+      </c>
+      <c r="P6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>-2.84520843</v>
+      </c>
+      <c r="C7">
+        <v>0.89073910000000001</v>
+      </c>
+      <c r="D7">
+        <v>4.1514751099999998</v>
+      </c>
+      <c r="F7" t="s">
+        <v>202</v>
+      </c>
+      <c r="K7" t="s">
+        <v>202</v>
+      </c>
+      <c r="P7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>-1.3366315499999999</v>
+      </c>
+      <c r="C8">
+        <v>1.53179983</v>
+      </c>
+      <c r="D8">
+        <v>3.4752312000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>203</v>
+      </c>
+      <c r="K8" t="s">
+        <v>203</v>
+      </c>
+      <c r="P8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>-2.5802639900000002</v>
+      </c>
+      <c r="C9">
+        <v>0.47248098999999999</v>
+      </c>
+      <c r="D9">
+        <v>2.0401646000000002</v>
+      </c>
+      <c r="F9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K9" t="s">
+        <v>204</v>
+      </c>
+      <c r="P9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>-3.41571772</v>
+      </c>
+      <c r="C10">
+        <v>1.6556706999999999</v>
+      </c>
+      <c r="D10">
+        <v>1.5785370299999999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>205</v>
+      </c>
+      <c r="K10" t="s">
+        <v>205</v>
+      </c>
+      <c r="P10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>-2.8408813999999998</v>
+      </c>
+      <c r="C11">
+        <v>2.5834136999999999</v>
+      </c>
+      <c r="D11">
+        <v>1.62685641</v>
+      </c>
+      <c r="F11" t="s">
+        <v>206</v>
+      </c>
+      <c r="K11" t="s">
+        <v>206</v>
+      </c>
+      <c r="P11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>-4.2984314000000001</v>
+      </c>
+      <c r="C12">
+        <v>1.77881355</v>
+      </c>
+      <c r="D12">
+        <v>2.2144044100000002</v>
+      </c>
+      <c r="F12" t="s">
+        <v>207</v>
+      </c>
+      <c r="K12" t="s">
+        <v>207</v>
+      </c>
+      <c r="P12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>-3.7534316200000002</v>
+      </c>
+      <c r="C13">
+        <v>1.5153502400000001</v>
+      </c>
+      <c r="D13">
+        <v>0.54797812999999995</v>
+      </c>
+      <c r="F13" t="s">
+        <v>208</v>
+      </c>
+      <c r="K13" t="s">
+        <v>208</v>
+      </c>
+      <c r="P13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>-3.3582180899999998</v>
+      </c>
+      <c r="C14">
+        <v>-0.84951829999999995</v>
+      </c>
+      <c r="D14">
+        <v>1.9587014700000001</v>
+      </c>
+      <c r="F14" t="s">
+        <v>209</v>
+      </c>
+      <c r="K14" t="s">
+        <v>209</v>
+      </c>
+      <c r="P14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>-3.6969055900000001</v>
+      </c>
+      <c r="C15">
+        <v>-1.22527271</v>
+      </c>
+      <c r="D15">
+        <v>2.9254328200000002</v>
+      </c>
+      <c r="F15" t="s">
+        <v>210</v>
+      </c>
+      <c r="K15" t="s">
+        <v>210</v>
+      </c>
+      <c r="P15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>-4.2102951400000004</v>
+      </c>
+      <c r="C16">
+        <v>-0.79377538999999997</v>
+      </c>
+      <c r="D16">
+        <v>1.27204333</v>
+      </c>
+      <c r="F16" t="s">
+        <v>211</v>
+      </c>
+      <c r="K16" t="s">
+        <v>211</v>
+      </c>
+      <c r="P16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>-1.42430766</v>
+      </c>
+      <c r="C17">
+        <v>-1.0717599499999999</v>
+      </c>
+      <c r="D17">
+        <v>0.86894534999999995</v>
+      </c>
+      <c r="F17" t="s">
+        <v>212</v>
+      </c>
+      <c r="K17" t="s">
+        <v>212</v>
+      </c>
+      <c r="P17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>0.84463270000000001</v>
+      </c>
+      <c r="C18">
+        <v>1.5645013699999999</v>
+      </c>
+      <c r="D18">
+        <v>-3.2536082999999998</v>
+      </c>
+      <c r="F18" t="s">
+        <v>213</v>
+      </c>
+      <c r="K18" t="s">
+        <v>213</v>
+      </c>
+      <c r="P18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>0.95358721000000002</v>
+      </c>
+      <c r="C19">
+        <v>2.4716466600000002</v>
+      </c>
+      <c r="D19">
+        <v>-2.6548383800000002</v>
+      </c>
+      <c r="F19" t="s">
+        <v>214</v>
+      </c>
+      <c r="K19" t="s">
+        <v>214</v>
+      </c>
+      <c r="P19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>0.78632484999999996</v>
+      </c>
+      <c r="C20">
+        <v>1.86287881</v>
+      </c>
+      <c r="D20">
+        <v>-4.3057477000000004</v>
+      </c>
+      <c r="F20" t="s">
+        <v>215</v>
+      </c>
+      <c r="K20" t="s">
+        <v>215</v>
+      </c>
+      <c r="P20" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>1.7434746699999999</v>
+      </c>
+      <c r="C21">
+        <v>0.95600417000000004</v>
+      </c>
+      <c r="D21">
+        <v>-3.1204059700000002</v>
+      </c>
+      <c r="F21" t="s">
+        <v>216</v>
+      </c>
+      <c r="K21" t="s">
+        <v>216</v>
+      </c>
+      <c r="P21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>-0.3989393</v>
+      </c>
+      <c r="C22">
+        <v>0.78359533999999997</v>
+      </c>
+      <c r="D22">
+        <v>-2.8507298599999999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>217</v>
+      </c>
+      <c r="K22" t="s">
+        <v>217</v>
+      </c>
+      <c r="P22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>-1.6521990200000001</v>
+      </c>
+      <c r="C23">
+        <v>1.6426283800000001</v>
+      </c>
+      <c r="D23">
+        <v>-2.9855547800000002</v>
+      </c>
+      <c r="F23" t="s">
+        <v>218</v>
+      </c>
+      <c r="K23" t="s">
+        <v>218</v>
+      </c>
+      <c r="P23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>-2.5411950499999998</v>
+      </c>
+      <c r="C24">
+        <v>1.0822184699999999</v>
+      </c>
+      <c r="D24">
+        <v>-2.6820371999999999</v>
+      </c>
+      <c r="F24" t="s">
+        <v>219</v>
+      </c>
+      <c r="K24" t="s">
+        <v>219</v>
+      </c>
+      <c r="P24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>-1.78834589</v>
+      </c>
+      <c r="C25">
+        <v>1.96629846</v>
+      </c>
+      <c r="D25">
+        <v>-4.02274362</v>
+      </c>
+      <c r="F25" t="s">
+        <v>220</v>
+      </c>
+      <c r="K25" t="s">
+        <v>220</v>
+      </c>
+      <c r="P25" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>-1.57746699</v>
+      </c>
+      <c r="C26">
+        <v>2.53641278</v>
+      </c>
+      <c r="D26">
+        <v>-2.36117446</v>
+      </c>
+      <c r="F26" t="s">
+        <v>221</v>
+      </c>
+      <c r="K26" t="s">
+        <v>221</v>
+      </c>
+      <c r="P26" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>-0.52638600999999996</v>
+      </c>
+      <c r="C27">
+        <v>-0.53760218999999998</v>
+      </c>
+      <c r="D27">
+        <v>-3.6369934599999998</v>
+      </c>
+      <c r="F27" t="s">
+        <v>222</v>
+      </c>
+      <c r="K27" t="s">
+        <v>222</v>
+      </c>
+      <c r="P27" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>-1.4432126700000001</v>
+      </c>
+      <c r="C28">
+        <v>-0.60385568000000001</v>
+      </c>
+      <c r="D28">
+        <v>-4.2275911400000004</v>
+      </c>
+      <c r="F28" t="s">
+        <v>223</v>
+      </c>
+      <c r="K28" t="s">
+        <v>223</v>
+      </c>
+      <c r="P28" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>0.33189657</v>
+      </c>
+      <c r="C29">
+        <v>-0.73049620000000004</v>
+      </c>
+      <c r="D29">
+        <v>-4.2866518200000003</v>
+      </c>
+      <c r="F29" t="s">
+        <v>224</v>
+      </c>
+      <c r="K29" t="s">
+        <v>224</v>
+      </c>
+      <c r="P29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>-0.3886096</v>
+      </c>
+      <c r="C30">
+        <v>-0.98677168999999998</v>
+      </c>
+      <c r="D30">
+        <v>-1.4408494599999999</v>
+      </c>
+      <c r="F30" t="s">
+        <v>225</v>
+      </c>
+      <c r="K30" t="s">
+        <v>225</v>
+      </c>
+      <c r="P30" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>3.2937205899999999</v>
+      </c>
+      <c r="C31">
+        <v>0.63657680999999999</v>
+      </c>
+      <c r="D31">
+        <v>2.3144055699999999</v>
+      </c>
+      <c r="F31" t="s">
+        <v>226</v>
+      </c>
+      <c r="K31" t="s">
+        <v>226</v>
+      </c>
+      <c r="P31" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>3.1575887100000002</v>
+      </c>
+      <c r="C32">
+        <v>1.70162334</v>
+      </c>
+      <c r="D32">
+        <v>2.1194169999999999</v>
+      </c>
+      <c r="F32" t="s">
+        <v>227</v>
+      </c>
+      <c r="K32" t="s">
+        <v>227</v>
+      </c>
+      <c r="P32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>4.3298833999999999</v>
+      </c>
+      <c r="C33">
+        <v>0.48817368999999999</v>
+      </c>
+      <c r="D33">
+        <v>2.6363900600000001</v>
+      </c>
+      <c r="F33" t="s">
+        <v>228</v>
+      </c>
+      <c r="K33" t="s">
+        <v>228</v>
+      </c>
+      <c r="P33" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>2.6346573100000001</v>
+      </c>
+      <c r="C34">
+        <v>0.35726848999999999</v>
+      </c>
+      <c r="D34">
+        <v>3.14056202</v>
+      </c>
+      <c r="F34" t="s">
+        <v>229</v>
+      </c>
+      <c r="K34" t="s">
+        <v>229</v>
+      </c>
+      <c r="P34" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>2.9983885199999998</v>
+      </c>
+      <c r="C35">
+        <v>-0.20076206999999999</v>
+      </c>
+      <c r="D35">
+        <v>1.0792377099999999</v>
+      </c>
+      <c r="F35" t="s">
+        <v>230</v>
+      </c>
+      <c r="K35" t="s">
+        <v>230</v>
+      </c>
+      <c r="P35" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>3.82464103</v>
+      </c>
+      <c r="C36">
+        <v>0.26684225</v>
+      </c>
+      <c r="D36">
+        <v>-0.1171201</v>
+      </c>
+      <c r="F36" t="s">
+        <v>231</v>
+      </c>
+      <c r="K36" t="s">
+        <v>231</v>
+      </c>
+      <c r="P36" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>3.6718260300000001</v>
+      </c>
+      <c r="C37">
+        <v>-0.39571588000000002</v>
+      </c>
+      <c r="D37">
+        <v>-0.97414729</v>
+      </c>
+      <c r="F37" t="s">
+        <v>232</v>
+      </c>
+      <c r="K37" t="s">
+        <v>232</v>
+      </c>
+      <c r="P37" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>4.8928892299999998</v>
+      </c>
+      <c r="C38">
+        <v>0.27347111000000002</v>
+      </c>
+      <c r="D38">
+        <v>0.12424092</v>
+      </c>
+      <c r="F38" t="s">
+        <v>233</v>
+      </c>
+      <c r="K38" t="s">
+        <v>233</v>
+      </c>
+      <c r="P38" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>3.5335902199999998</v>
+      </c>
+      <c r="C39">
+        <v>1.27579295</v>
+      </c>
+      <c r="D39">
+        <v>-0.41912891000000002</v>
+      </c>
+      <c r="F39" t="s">
+        <v>234</v>
+      </c>
+      <c r="K39" t="s">
+        <v>234</v>
+      </c>
+      <c r="P39" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>3.2125176099999999</v>
+      </c>
+      <c r="C40">
+        <v>-1.69851982</v>
+      </c>
+      <c r="D40">
+        <v>1.3561398499999999</v>
+      </c>
+      <c r="F40" t="s">
+        <v>235</v>
+      </c>
+      <c r="K40" t="s">
+        <v>235</v>
+      </c>
+      <c r="P40" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>4.1043784600000004</v>
+      </c>
+      <c r="C41">
+        <v>-2.1141078000000002</v>
+      </c>
+      <c r="D41">
+        <v>0.88339460999999997</v>
+      </c>
+      <c r="F41" t="s">
+        <v>236</v>
+      </c>
+      <c r="K41" t="s">
+        <v>236</v>
+      </c>
+      <c r="P41" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>3.2336552900000002</v>
+      </c>
+      <c r="C42">
+        <v>-1.9278925600000001</v>
+      </c>
+      <c r="D42">
+        <v>2.4270357699999998</v>
+      </c>
+      <c r="F42" t="s">
+        <v>237</v>
+      </c>
+      <c r="K42" t="s">
+        <v>237</v>
+      </c>
+      <c r="P42" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>1.1590300200000001</v>
+      </c>
+      <c r="C43">
+        <v>-1.3802196200000001</v>
+      </c>
+      <c r="D43">
+        <v>0.53258587999999996</v>
+      </c>
+      <c r="F43" t="s">
+        <v>238</v>
+      </c>
+      <c r="K43" t="s">
+        <v>238</v>
+      </c>
+      <c r="P43" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>-0.51999039999999996</v>
+      </c>
+      <c r="C44">
+        <v>-3.4218376300000002</v>
+      </c>
+      <c r="D44">
+        <v>-6.233851E-2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>239</v>
+      </c>
+      <c r="K44" t="s">
+        <v>239</v>
+      </c>
+      <c r="P44" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>-0.89046018000000005</v>
+      </c>
+      <c r="C45">
+        <v>-4.1741158699999996</v>
+      </c>
+      <c r="D45">
+        <v>-1.1826825599999999</v>
+      </c>
+      <c r="F45" t="s">
+        <v>240</v>
+      </c>
+      <c r="K45" t="s">
+        <v>240</v>
+      </c>
+      <c r="P45" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>-1.02570988</v>
+      </c>
+      <c r="C46">
+        <v>-3.68213517</v>
+      </c>
+      <c r="D46">
+        <v>-2.1386323900000002</v>
+      </c>
+      <c r="F46" t="s">
+        <v>241</v>
+      </c>
+      <c r="K46" t="s">
+        <v>241</v>
+      </c>
+      <c r="P46" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>-1.08971493</v>
+      </c>
+      <c r="C47">
+        <v>-5.5516549199999998</v>
+      </c>
+      <c r="D47">
+        <v>-1.11062255</v>
+      </c>
+      <c r="F47" t="s">
+        <v>242</v>
+      </c>
+      <c r="K47" t="s">
+        <v>242</v>
+      </c>
+      <c r="P47" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>-1.37601489</v>
+      </c>
+      <c r="C48">
+        <v>-6.09995098</v>
+      </c>
+      <c r="D48">
+        <v>-2.0048662300000002</v>
+      </c>
+      <c r="F48" t="s">
+        <v>243</v>
+      </c>
+      <c r="K48" t="s">
+        <v>243</v>
+      </c>
+      <c r="P48" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>-0.9261568</v>
+      </c>
+      <c r="C49">
+        <v>-6.2236605599999999</v>
+      </c>
+      <c r="D49">
+        <v>9.2842430000000004E-2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>244</v>
+      </c>
+      <c r="K49" t="s">
+        <v>244</v>
+      </c>
+      <c r="P49" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>-1.08049076</v>
+      </c>
+      <c r="C50">
+        <v>-7.2978599700000002</v>
+      </c>
+      <c r="D50">
+        <v>0.15070475999999999</v>
+      </c>
+      <c r="F50" t="s">
+        <v>245</v>
+      </c>
+      <c r="K50" t="s">
+        <v>245</v>
+      </c>
+      <c r="P50" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>-0.56161804000000004</v>
+      </c>
+      <c r="C51">
+        <v>-5.5010464900000002</v>
+      </c>
+      <c r="D51">
+        <v>1.2248054399999999</v>
+      </c>
+      <c r="F51" t="s">
+        <v>246</v>
+      </c>
+      <c r="K51" t="s">
+        <v>246</v>
+      </c>
+      <c r="P51" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>-0.43036148000000002</v>
+      </c>
+      <c r="C52">
+        <v>-6.0094153700000001</v>
+      </c>
+      <c r="D52">
+        <v>2.1768264400000001</v>
+      </c>
+      <c r="F52" t="s">
+        <v>247</v>
+      </c>
+      <c r="K52" t="s">
+        <v>247</v>
+      </c>
+      <c r="P52" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>-0.36559821999999997</v>
+      </c>
+      <c r="C53">
+        <v>-4.1291235100000003</v>
+      </c>
+      <c r="D53">
+        <v>1.1395707500000001</v>
+      </c>
+      <c r="F53" t="s">
+        <v>248</v>
+      </c>
+      <c r="K53" t="s">
+        <v>248</v>
+      </c>
+      <c r="P53" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>-8.1234150000000005E-2</v>
+      </c>
+      <c r="C54">
+        <v>-3.5922666099999998</v>
+      </c>
+      <c r="D54">
+        <v>2.04220259</v>
+      </c>
+      <c r="F54" t="s">
+        <v>249</v>
+      </c>
+      <c r="K54" t="s">
+        <v>249</v>
+      </c>
+      <c r="P54" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="6">
+        <v>0.27978106000000003</v>
+      </c>
+      <c r="C55" s="6">
+        <v>2.7561179099999999</v>
+      </c>
+      <c r="D55" s="6">
+        <v>1.6492811199999999</v>
+      </c>
+      <c r="E55" s="6"/>
+      <c r="F55" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="K55" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="P55" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="6">
+        <v>-0.64361374999999998</v>
+      </c>
+      <c r="C56" s="6">
+        <v>3.0675661600000002</v>
+      </c>
+      <c r="D56" s="6">
+        <v>2.1428520600000001</v>
+      </c>
+      <c r="E56" s="6"/>
+      <c r="F56" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="K56" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="P56" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="6">
+        <v>1.07797371</v>
+      </c>
+      <c r="C57" s="6">
+        <v>2.6340478699999998</v>
+      </c>
+      <c r="D57" s="6">
+        <v>2.38262792</v>
+      </c>
+      <c r="E57" s="6"/>
+      <c r="F57" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="K57" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="P57" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="5"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="6">
+        <v>0.61625132000000005</v>
+      </c>
+      <c r="C58" s="6">
+        <v>3.5982463999999998</v>
+      </c>
+      <c r="D58" s="6">
+        <v>0.50504998999999995</v>
+      </c>
+      <c r="E58" s="6"/>
+      <c r="F58" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="K58" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="P58" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="6">
+        <v>-0.39609545000000002</v>
+      </c>
+      <c r="C59" s="6">
+        <v>4.2214214500000002</v>
+      </c>
+      <c r="D59" s="6">
+        <v>-0.26517851999999997</v>
+      </c>
+      <c r="E59" s="6"/>
+      <c r="F59" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="K59" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="P59" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="6">
+        <v>-1.42613089</v>
+      </c>
+      <c r="C60" s="6">
+        <v>4.1613802499999997</v>
+      </c>
+      <c r="D60" s="6">
+        <v>7.9842129999999997E-2</v>
+      </c>
+      <c r="E60" s="6"/>
+      <c r="F60" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="K60" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="P60" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="5"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="6">
+        <v>-9.8754400000000006E-2</v>
+      </c>
+      <c r="C61" s="6">
+        <v>4.9578781200000002</v>
+      </c>
+      <c r="D61" s="6">
+        <v>-1.4025905599999999</v>
+      </c>
+      <c r="E61" s="6"/>
+      <c r="F61" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="K61" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="P61" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="6">
+        <v>-0.90107378000000005</v>
+      </c>
+      <c r="C62" s="6">
+        <v>5.4459774400000001</v>
+      </c>
+      <c r="D62" s="6">
+        <v>-1.9495838000000001</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="F62" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="K62" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="P62" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="6">
+        <v>1.2184429800000001</v>
+      </c>
+      <c r="C63" s="6">
+        <v>5.0893853699999996</v>
+      </c>
+      <c r="D63" s="6">
+        <v>-1.8369052699999999</v>
+      </c>
+      <c r="E63" s="6"/>
+      <c r="F63" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="K63" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="P63" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="6">
+        <v>1.45116925</v>
+      </c>
+      <c r="C64" s="6">
+        <v>5.6734304299999998</v>
+      </c>
+      <c r="D64" s="6">
+        <v>-2.7218331199999999</v>
+      </c>
+      <c r="E64" s="6"/>
+      <c r="F64" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="K64" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="P64" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q64" s="5"/>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="6">
+        <v>2.23141743</v>
+      </c>
+      <c r="C65" s="6">
+        <v>4.4640636599999999</v>
+      </c>
+      <c r="D65" s="6">
+        <v>-1.1171684</v>
+      </c>
+      <c r="E65" s="6"/>
+      <c r="F65" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="K65" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="P65" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q65" s="5"/>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="6">
+        <v>3.2645103799999999</v>
+      </c>
+      <c r="C66" s="6">
+        <v>4.5617077699999999</v>
+      </c>
+      <c r="D66" s="6">
+        <v>-1.4398491499999999</v>
+      </c>
+      <c r="E66" s="6"/>
+      <c r="F66" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="K66" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="P66" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q66" s="5"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A67" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="6">
+        <v>1.9379836800000001</v>
+      </c>
+      <c r="C67" s="6">
+        <v>3.7264337799999998</v>
+      </c>
+      <c r="D67" s="6">
+        <v>2.2798840000000001E-2</v>
+      </c>
+      <c r="E67" s="6"/>
+      <c r="F67" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="K67" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="P67" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5"/>
+      <c r="S67" s="5"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="6">
+        <v>2.7488137199999998</v>
+      </c>
+      <c r="C68" s="6">
+        <v>3.28943553</v>
+      </c>
+      <c r="D68" s="6">
+        <v>0.59797171000000005</v>
+      </c>
+      <c r="E68" s="6"/>
+      <c r="F68" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="K68" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="P68" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69">
+        <v>-1.4670704000000001</v>
+      </c>
+      <c r="C69">
+        <v>0.19585760999999999</v>
+      </c>
+      <c r="D69">
+        <v>1.1050858699999999</v>
+      </c>
+      <c r="F69" t="s">
+        <v>264</v>
+      </c>
+      <c r="K69" t="s">
+        <v>264</v>
+      </c>
+      <c r="P69" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>-0.27456888000000002</v>
+      </c>
+      <c r="C70">
+        <v>0.29352719999999999</v>
+      </c>
+      <c r="D70">
+        <v>-1.46418381</v>
+      </c>
+      <c r="F70" t="s">
+        <v>265</v>
+      </c>
+      <c r="K70" t="s">
+        <v>265</v>
+      </c>
+      <c r="P70" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71">
+        <v>1.56698062</v>
+      </c>
+      <c r="C71">
+        <v>-0.17029783000000001</v>
+      </c>
+      <c r="D71">
+        <v>0.71056412000000002</v>
+      </c>
+      <c r="F71" t="s">
+        <v>266</v>
+      </c>
+      <c r="K71" t="s">
+        <v>266</v>
+      </c>
+      <c r="P71" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>-0.56461344000000002</v>
+      </c>
+      <c r="C72">
+        <v>-1.5685956700000001</v>
+      </c>
+      <c r="D72">
+        <v>-2.6399185699999999</v>
+      </c>
+      <c r="F72" t="s">
+        <v>267</v>
+      </c>
+      <c r="K72" t="s">
+        <v>267</v>
+      </c>
+      <c r="P72" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>-2.41878927</v>
+      </c>
+      <c r="C73">
+        <v>-1.78692951</v>
+      </c>
+      <c r="D73">
+        <v>1.4160822900000001</v>
+      </c>
+      <c r="F73" t="s">
+        <v>268</v>
+      </c>
+      <c r="K73" t="s">
+        <v>268</v>
+      </c>
+      <c r="P73" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>2.0634775799999998</v>
+      </c>
+      <c r="C74">
+        <v>-2.33967167</v>
+      </c>
+      <c r="D74">
+        <v>0.79187686999999995</v>
+      </c>
+      <c r="F74" t="s">
+        <v>269</v>
+      </c>
+      <c r="K74" t="s">
+        <v>269</v>
+      </c>
+      <c r="P74" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>